<commit_message>
Optimize project structure by centralizing parameters in config.py" -m "This commit introduces significant improvements to the project structure by centralizing all configuration parameters in the config.py file. The main changes include:
1. Moved all hardcoded parameters from main.py, login.py, and other modules to config.py.
2. Updated main(), login(), and other relevant functions to use parameters from config.py.
3. Improved code maintainability and flexibility by centralizing configuration.
4. Enhanced readability by removing hardcoded values from function bodies.
5. Simplified future updates by providing a single point of configuration.

Key updates:
- Added EXCEL_FILE_NAME, EXCEL_SHEET_NAME, and EXCEL_FILE_PATH to config.py for Excel file handling.
- Moved login-related parameters (URLs, selectors, credentials) to config.py.
- Centralized WebDriver configuration options in config.py.
- Updated import statements in affected files to use new config parameters.
</commit_message>
<xml_diff>
--- a/afisha.xlsx
+++ b/afisha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergej/StudioProjects/Egolist/egolist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5855C0A0-FD99-984A-B57C-03E5C8F54582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315D354B-E362-B845-8453-279FEA53B335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{C580A3C3-98DD-0143-B76E-E77FC3D5C218}"/>
+    <workbookView xWindow="-36180" yWindow="840" windowWidth="34560" windowHeight="19880" xr2:uid="{C580A3C3-98DD-0143-B76E-E77FC3D5C218}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Отметка о публикации</t>
   </si>
@@ -77,78 +77,13 @@
   </si>
   <si>
     <t>Видео URL 1</t>
-  </si>
-  <si>
-    <t>Майстер-класи</t>
-  </si>
-  <si>
-    <t>Безкоштовно</t>
-  </si>
-  <si>
-    <t>Дніпро</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
-    <t>м. Дніпро</t>
-  </si>
-  <si>
-    <t>Активний відпочинок</t>
-  </si>
-  <si>
-    <t>В цю суботу 21 вересня з 17:00 до 20:00  танцюємо, заряджаємо позитивними емоціями та гарним настроєм 🤩! 
-Цього разу вечірка для тих, хто вважає, що буде 52 серпня. Тих, кому ще мало було літа і хочеться продовження. Для тих, в кого ще продовжується літо.</t>
-  </si>
-  <si>
-    <t>ДРЕСС-КОД: літній одяг 
-В нас працюють відеографи 📸 Video Shaika і будуть чудові фото та відео 😎!!! 
-💃 Танцюємо: 
-- Salsa 
-- Zouk 
-- Bachata 
-- Kizomba 
---Rueda de Casino</t>
-  </si>
-  <si>
-    <t>Latina Party in Dnipro</t>
-  </si>
-  <si>
-    <t>м. Дніпро, вул. Яворницького 57, 5 пов./зала 512</t>
-  </si>
-  <si>
-    <t>https://t.me/ZUEVDANCE</t>
-  </si>
-  <si>
-    <t>(098) 065 85 58</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/r3d2k6w/12.jpg</t>
-  </si>
-  <si>
-    <t>Більшість IT-компаній втрачають великі гроші через банальні помилки у плануванні та бюджетуванні. Як уникнути фатальних помилок в IT? 
-Зануритись у світ фінансів в IT допоможе Петро Яворський — Lead Financial Partner at Luxoft на безкоштовній онлайн лекції</t>
-  </si>
-  <si>
-    <t>Про що розкажуть: 
-✔️ Важливість планування та основні користувачі фінансової інформації 
-✔️ Специфіка роботи з фінансами в інформаційному бізнесі 
-✔️ Релевантні фінансові показники: виручка, витрати, маржа, показники ліквідності та інше 
-✔️ Як правильно зробити прогнози доходів та витрат 
-✔️ Розберемо фатальні помилки при складанні бюджетів</t>
-  </si>
-  <si>
-    <t>https://bit.ly/3ZtTsPp</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/bgbRbHG/6.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,21 +126,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -224,35 +144,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,16 +482,17 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
     <col min="3" max="3" width="70.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -622,94 +537,12 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="6">
-        <v>200</v>
-      </c>
-      <c r="F2" s="8">
-        <v>45556</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="6"/>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="8">
-        <v>45584</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="6"/>
+      <c r="A3" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{FA15ADA4-9804-B94D-978F-1D8D0729A0A3}"/>
-    <hyperlink ref="M2" r:id="rId2" xr:uid="{CB83C0F6-A199-A44F-862B-8F65A24AA627}"/>
-    <hyperlink ref="K3" r:id="rId3" xr:uid="{AA5F87D9-96FD-254D-BF4D-53B541F97C4B}"/>
-    <hyperlink ref="M3" r:id="rId4" xr:uid="{105F9D06-EE85-B247-8205-6E7DE885EDD6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>